<commit_message>
replace datasets with most recent version
</commit_message>
<xml_diff>
--- a/data/Table_1.4a_Primary_Energy_Imports_by_Source.xlsx
+++ b/data/Table_1.4a_Primary_Energy_Imports_by_Source.xlsx
@@ -21,13 +21,13 @@
     <t>U.S. Energy Information Administration</t>
   </si>
   <si>
-    <t>July 2018 Monthly Energy Review</t>
+    <t>July 2020 Monthly Energy Review</t>
   </si>
   <si>
-    <t>Release Date: July 26, 2018</t>
+    <t>Release Date: July 28, 2020</t>
   </si>
   <si>
-    <t>Next Update: August 28, 2018</t>
+    <t>Next Update: August 26, 2020</t>
   </si>
   <si>
     <t>Table 1.4a Primary Energy Imports by Source</t>
@@ -476,7 +476,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J556"/>
+  <dimension ref="A1:J580"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -17490,7 +17490,7 @@
         <v>42736</v>
       </c>
       <c r="B541">
-        <v>0.015962</v>
+        <v>0.015968</v>
       </c>
       <c r="C541">
         <v>9.0E-6</v>
@@ -17499,13 +17499,13 @@
         <v>0.298948</v>
       </c>
       <c r="E541">
-        <v>1.584933</v>
+        <v>1.590007</v>
       </c>
       <c r="F541">
-        <v>0.380237</v>
+        <v>0.383014</v>
       </c>
       <c r="G541">
-        <v>1.96517</v>
+        <v>1.973021</v>
       </c>
       <c r="H541">
         <v>0.002791</v>
@@ -17514,7 +17514,7 @@
         <v>0.023947</v>
       </c>
       <c r="J541">
-        <v>2.306828</v>
+        <v>2.314684</v>
       </c>
     </row>
     <row r="542" spans="1:10">
@@ -17522,7 +17522,7 @@
         <v>42767</v>
       </c>
       <c r="B542">
-        <v>0.013152</v>
+        <v>0.013158</v>
       </c>
       <c r="C542">
         <v>1.5E-5</v>
@@ -17531,13 +17531,13 @@
         <v>0.260962</v>
       </c>
       <c r="E542">
-        <v>1.338911</v>
+        <v>1.334376</v>
       </c>
       <c r="F542">
-        <v>0.326253</v>
+        <v>0.327088</v>
       </c>
       <c r="G542">
-        <v>1.665165</v>
+        <v>1.661464</v>
       </c>
       <c r="H542">
         <v>0.004299</v>
@@ -17546,7 +17546,7 @@
         <v>0.019354</v>
       </c>
       <c r="J542">
-        <v>1.962947</v>
+        <v>1.959252</v>
       </c>
     </row>
     <row r="543" spans="1:10">
@@ -17554,7 +17554,7 @@
         <v>42795</v>
       </c>
       <c r="B543">
-        <v>0.012022</v>
+        <v>0.012027</v>
       </c>
       <c r="C543">
         <v>1.0E-5</v>
@@ -17563,13 +17563,13 @@
         <v>0.287582</v>
       </c>
       <c r="E543">
-        <v>1.512226</v>
+        <v>1.53134</v>
       </c>
       <c r="F543">
-        <v>0.336377</v>
+        <v>0.337491</v>
       </c>
       <c r="G543">
-        <v>1.848603</v>
+        <v>1.868831</v>
       </c>
       <c r="H543">
         <v>0.005989</v>
@@ -17578,7 +17578,7 @@
         <v>0.020551</v>
       </c>
       <c r="J543">
-        <v>2.174755</v>
+        <v>2.194988</v>
       </c>
     </row>
     <row r="544" spans="1:10">
@@ -17586,7 +17586,7 @@
         <v>42826</v>
       </c>
       <c r="B544">
-        <v>0.010587</v>
+        <v>0.010591</v>
       </c>
       <c r="C544">
         <v>4.8E-5</v>
@@ -17595,13 +17595,13 @@
         <v>0.244236</v>
       </c>
       <c r="E544">
-        <v>1.478411</v>
+        <v>1.489099</v>
       </c>
       <c r="F544">
-        <v>0.341722</v>
+        <v>0.342333</v>
       </c>
       <c r="G544">
-        <v>1.820133</v>
+        <v>1.831432</v>
       </c>
       <c r="H544">
         <v>0.006427</v>
@@ -17610,7 +17610,7 @@
         <v>0.018978</v>
       </c>
       <c r="J544">
-        <v>2.100409</v>
+        <v>2.111712</v>
       </c>
     </row>
     <row r="545" spans="1:10">
@@ -17618,7 +17618,7 @@
         <v>42856</v>
       </c>
       <c r="B545">
-        <v>0.022621</v>
+        <v>0.02263</v>
       </c>
       <c r="C545">
         <v>1.4E-5</v>
@@ -17627,13 +17627,13 @@
         <v>0.250462</v>
       </c>
       <c r="E545">
-        <v>1.577812</v>
+        <v>1.591791</v>
       </c>
       <c r="F545">
-        <v>0.371936</v>
+        <v>0.373704</v>
       </c>
       <c r="G545">
-        <v>1.949747</v>
+        <v>1.965495</v>
       </c>
       <c r="H545">
         <v>0.007814</v>
@@ -17642,7 +17642,7 @@
         <v>0.017347</v>
       </c>
       <c r="J545">
-        <v>2.248005</v>
+        <v>2.263762</v>
       </c>
     </row>
     <row r="546" spans="1:10">
@@ -17650,7 +17650,7 @@
         <v>42887</v>
       </c>
       <c r="B546">
-        <v>0.013985</v>
+        <v>0.013991</v>
       </c>
       <c r="C546">
         <v>0.000611</v>
@@ -17659,13 +17659,13 @@
         <v>0.2458</v>
       </c>
       <c r="E546">
-        <v>1.456507</v>
+        <v>1.468196</v>
       </c>
       <c r="F546">
-        <v>0.354598</v>
+        <v>0.355496</v>
       </c>
       <c r="G546">
-        <v>1.811105</v>
+        <v>1.823691</v>
       </c>
       <c r="H546">
         <v>0.012718</v>
@@ -17674,7 +17674,7 @@
         <v>0.020448</v>
       </c>
       <c r="J546">
-        <v>2.104667</v>
+        <v>2.117259</v>
       </c>
     </row>
     <row r="547" spans="1:10">
@@ -17682,7 +17682,7 @@
         <v>42917</v>
       </c>
       <c r="B547">
-        <v>0.020541</v>
+        <v>0.020549</v>
       </c>
       <c r="C547">
         <v>4.6E-5</v>
@@ -17691,13 +17691,13 @@
         <v>0.256771</v>
       </c>
       <c r="E547">
-        <v>1.470277</v>
+        <v>1.484482</v>
       </c>
       <c r="F547">
-        <v>0.332596</v>
+        <v>0.334921</v>
       </c>
       <c r="G547">
-        <v>1.802873</v>
+        <v>1.819404</v>
       </c>
       <c r="H547">
         <v>0.01206</v>
@@ -17706,7 +17706,7 @@
         <v>0.020176</v>
       </c>
       <c r="J547">
-        <v>2.112467</v>
+        <v>2.129007</v>
       </c>
     </row>
     <row r="548" spans="1:10">
@@ -17714,7 +17714,7 @@
         <v>42948</v>
       </c>
       <c r="B548">
-        <v>0.018019</v>
+        <v>0.018027</v>
       </c>
       <c r="C548">
         <v>4.8E-5</v>
@@ -17723,13 +17723,13 @@
         <v>0.254085</v>
       </c>
       <c r="E548">
-        <v>1.48249</v>
+        <v>1.485947</v>
       </c>
       <c r="F548">
-        <v>0.357151</v>
+        <v>0.361154</v>
       </c>
       <c r="G548">
-        <v>1.839641</v>
+        <v>1.847101</v>
       </c>
       <c r="H548">
         <v>0.011406</v>
@@ -17738,7 +17738,7 @@
         <v>0.022208</v>
       </c>
       <c r="J548">
-        <v>2.145408</v>
+        <v>2.152875</v>
       </c>
     </row>
     <row r="549" spans="1:10">
@@ -17746,31 +17746,31 @@
         <v>42979</v>
       </c>
       <c r="B549">
-        <v>0.011015</v>
+        <v>0.01102</v>
       </c>
       <c r="C549">
         <v>2.6E-5</v>
       </c>
       <c r="D549">
-        <v>0.235219</v>
+        <v>0.23518</v>
       </c>
       <c r="E549">
-        <v>1.322886</v>
+        <v>1.329233</v>
       </c>
       <c r="F549">
-        <v>0.395171</v>
+        <v>0.395705</v>
       </c>
       <c r="G549">
-        <v>1.718057</v>
+        <v>1.724939</v>
       </c>
       <c r="H549">
-        <v>0.005465</v>
+        <v>0.004256</v>
       </c>
       <c r="I549">
         <v>0.017839</v>
       </c>
       <c r="J549">
-        <v>1.987621</v>
+        <v>1.99326</v>
       </c>
     </row>
     <row r="550" spans="1:10">
@@ -17778,22 +17778,22 @@
         <v>43009</v>
       </c>
       <c r="B550">
-        <v>0.012493</v>
+        <v>0.012498</v>
       </c>
       <c r="C550">
         <v>0.000282</v>
       </c>
       <c r="D550">
-        <v>0.250084</v>
+        <v>0.247371</v>
       </c>
       <c r="E550">
-        <v>1.430069</v>
+        <v>1.440559</v>
       </c>
       <c r="F550">
-        <v>0.344587</v>
+        <v>0.346093</v>
       </c>
       <c r="G550">
-        <v>1.774656</v>
+        <v>1.786652</v>
       </c>
       <c r="H550">
         <v>0.004435</v>
@@ -17802,7 +17802,7 @@
         <v>0.013486</v>
       </c>
       <c r="J550">
-        <v>2.055436</v>
+        <v>2.064724</v>
       </c>
     </row>
     <row r="551" spans="1:10">
@@ -17810,22 +17810,22 @@
         <v>43040</v>
       </c>
       <c r="B551">
-        <v>0.007896</v>
+        <v>0.007899</v>
       </c>
       <c r="C551">
         <v>0.000328</v>
       </c>
       <c r="D551">
-        <v>0.249773</v>
+        <v>0.246321</v>
       </c>
       <c r="E551">
-        <v>1.386169</v>
+        <v>1.392892</v>
       </c>
       <c r="F551">
-        <v>0.350937</v>
+        <v>0.357769</v>
       </c>
       <c r="G551">
-        <v>1.737106</v>
+        <v>1.750661</v>
       </c>
       <c r="H551">
         <v>0.004812</v>
@@ -17834,7 +17834,7 @@
         <v>0.013409</v>
       </c>
       <c r="J551">
-        <v>2.013325</v>
+        <v>2.023431</v>
       </c>
     </row>
     <row r="552" spans="1:10">
@@ -17842,22 +17842,22 @@
         <v>43070</v>
       </c>
       <c r="B552">
-        <v>0.008762</v>
+        <v>0.008766</v>
       </c>
       <c r="C552">
         <v>1.1E-5</v>
       </c>
       <c r="D552">
-        <v>0.28453</v>
+        <v>0.28134</v>
       </c>
       <c r="E552">
-        <v>1.462192</v>
+        <v>1.459532</v>
       </c>
       <c r="F552">
-        <v>0.361951</v>
+        <v>0.361981</v>
       </c>
       <c r="G552">
-        <v>1.824143</v>
+        <v>1.821513</v>
       </c>
       <c r="H552">
         <v>0.004344</v>
@@ -17866,7 +17866,7 @@
         <v>0.016374</v>
       </c>
       <c r="J552">
-        <v>2.138164</v>
+        <v>2.132348</v>
       </c>
     </row>
     <row r="553" spans="1:10">
@@ -17874,31 +17874,31 @@
         <v>43101</v>
       </c>
       <c r="B553">
-        <v>0.010732</v>
+        <v>0.0102</v>
       </c>
       <c r="C553">
         <v>5.1E-5</v>
       </c>
       <c r="D553">
-        <v>0.311146</v>
+        <v>0.307389</v>
       </c>
       <c r="E553">
-        <v>1.505455</v>
+        <v>1.506971</v>
       </c>
       <c r="F553">
-        <v>0.38094</v>
+        <v>0.380986</v>
       </c>
       <c r="G553">
-        <v>1.886396</v>
+        <v>1.887956</v>
       </c>
       <c r="H553">
         <v>0.004098</v>
       </c>
       <c r="I553">
-        <v>0.01854</v>
+        <v>0.017827</v>
       </c>
       <c r="J553">
-        <v>2.230963</v>
+        <v>2.227522</v>
       </c>
     </row>
     <row r="554" spans="1:10">
@@ -17906,31 +17906,31 @@
         <v>43132</v>
       </c>
       <c r="B554">
-        <v>0.007501</v>
+        <v>0.007129</v>
       </c>
       <c r="C554">
         <v>2.0E-6</v>
       </c>
       <c r="D554">
-        <v>0.246678</v>
+        <v>0.243352</v>
       </c>
       <c r="E554">
-        <v>1.271592</v>
+        <v>1.272878</v>
       </c>
       <c r="F554">
-        <v>0.318368</v>
+        <v>0.318348</v>
       </c>
       <c r="G554">
-        <v>1.58996</v>
+        <v>1.591226</v>
       </c>
       <c r="H554">
         <v>0.002634</v>
       </c>
       <c r="I554">
-        <v>0.016458</v>
+        <v>0.016336</v>
       </c>
       <c r="J554">
-        <v>1.863233</v>
+        <v>1.860679</v>
       </c>
     </row>
     <row r="555" spans="1:10">
@@ -17938,31 +17938,31 @@
         <v>43160</v>
       </c>
       <c r="B555">
-        <v>0.01113</v>
+        <v>0.010578</v>
       </c>
       <c r="C555">
         <v>5.1E-5</v>
       </c>
       <c r="D555">
-        <v>0.281143</v>
+        <v>0.277531</v>
       </c>
       <c r="E555">
-        <v>1.430917</v>
+        <v>1.432178</v>
       </c>
       <c r="F555">
-        <v>0.371501</v>
+        <v>0.370927</v>
       </c>
       <c r="G555">
-        <v>1.802418</v>
+        <v>1.803105</v>
       </c>
       <c r="H555">
         <v>0.00396</v>
       </c>
       <c r="I555">
-        <v>0.018115</v>
+        <v>0.019102</v>
       </c>
       <c r="J555">
-        <v>2.116817</v>
+        <v>2.114327</v>
       </c>
     </row>
     <row r="556" spans="1:10">
@@ -17970,31 +17970,799 @@
         <v>43191</v>
       </c>
       <c r="B556">
-        <v>0.010611</v>
+        <v>0.010085</v>
       </c>
       <c r="C556">
         <v>0.000562</v>
       </c>
       <c r="D556">
-        <v>0.249884</v>
+        <v>0.248321</v>
       </c>
       <c r="E556">
-        <v>1.499067</v>
+        <v>1.501247</v>
       </c>
       <c r="F556">
-        <v>0.345163</v>
+        <v>0.345352</v>
       </c>
       <c r="G556">
-        <v>1.84423</v>
+        <v>1.846599</v>
       </c>
       <c r="H556">
         <v>0.004101</v>
       </c>
       <c r="I556">
-        <v>0.016872</v>
+        <v>0.015452</v>
       </c>
       <c r="J556">
-        <v>2.12626</v>
+        <v>2.12512</v>
+      </c>
+    </row>
+    <row r="557" spans="1:10">
+      <c r="A557" s="6">
+        <v>43221</v>
+      </c>
+      <c r="B557">
+        <v>0.011101</v>
+      </c>
+      <c r="C557">
+        <v>0.000629</v>
+      </c>
+      <c r="D557">
+        <v>0.232847</v>
+      </c>
+      <c r="E557">
+        <v>1.472442</v>
+      </c>
+      <c r="F557">
+        <v>0.403652</v>
+      </c>
+      <c r="G557">
+        <v>1.876094</v>
+      </c>
+      <c r="H557">
+        <v>0.00361</v>
+      </c>
+      <c r="I557">
+        <v>0.017876</v>
+      </c>
+      <c r="J557">
+        <v>2.142157</v>
+      </c>
+    </row>
+    <row r="558" spans="1:10">
+      <c r="A558" s="6">
+        <v>43252</v>
+      </c>
+      <c r="B558">
+        <v>0.010383</v>
+      </c>
+      <c r="C558">
+        <v>0.000486</v>
+      </c>
+      <c r="D558">
+        <v>0.234181</v>
+      </c>
+      <c r="E558">
+        <v>1.543779</v>
+      </c>
+      <c r="F558">
+        <v>0.364964</v>
+      </c>
+      <c r="G558">
+        <v>1.908743</v>
+      </c>
+      <c r="H558">
+        <v>0.0038</v>
+      </c>
+      <c r="I558">
+        <v>0.018745</v>
+      </c>
+      <c r="J558">
+        <v>2.17634</v>
+      </c>
+    </row>
+    <row r="559" spans="1:10">
+      <c r="A559" s="6">
+        <v>43282</v>
+      </c>
+      <c r="B559">
+        <v>0.014127</v>
+      </c>
+      <c r="C559">
+        <v>7.0E-6</v>
+      </c>
+      <c r="D559">
+        <v>0.253187</v>
+      </c>
+      <c r="E559">
+        <v>1.491583</v>
+      </c>
+      <c r="F559">
+        <v>0.381853</v>
+      </c>
+      <c r="G559">
+        <v>1.873436</v>
+      </c>
+      <c r="H559">
+        <v>0.002369</v>
+      </c>
+      <c r="I559">
+        <v>0.018325</v>
+      </c>
+      <c r="J559">
+        <v>2.16145</v>
+      </c>
+    </row>
+    <row r="560" spans="1:10">
+      <c r="A560" s="6">
+        <v>43313</v>
+      </c>
+      <c r="B560">
+        <v>0.009878</v>
+      </c>
+      <c r="C560">
+        <v>2.8E-5</v>
+      </c>
+      <c r="D560">
+        <v>0.242951</v>
+      </c>
+      <c r="E560">
+        <v>1.501538</v>
+      </c>
+      <c r="F560">
+        <v>0.41129</v>
+      </c>
+      <c r="G560">
+        <v>1.912829</v>
+      </c>
+      <c r="H560">
+        <v>0.004894</v>
+      </c>
+      <c r="I560">
+        <v>0.020936</v>
+      </c>
+      <c r="J560">
+        <v>2.191516</v>
+      </c>
+    </row>
+    <row r="561" spans="1:10">
+      <c r="A561" s="6">
+        <v>43344</v>
+      </c>
+      <c r="B561">
+        <v>0.005366</v>
+      </c>
+      <c r="C561">
+        <v>0.00021</v>
+      </c>
+      <c r="D561">
+        <v>0.219426</v>
+      </c>
+      <c r="E561">
+        <v>1.381121</v>
+      </c>
+      <c r="F561">
+        <v>0.37479</v>
+      </c>
+      <c r="G561">
+        <v>1.755911</v>
+      </c>
+      <c r="H561">
+        <v>0.003386</v>
+      </c>
+      <c r="I561">
+        <v>0.014503</v>
+      </c>
+      <c r="J561">
+        <v>1.998803</v>
+      </c>
+    </row>
+    <row r="562" spans="1:10">
+      <c r="A562" s="6">
+        <v>43374</v>
+      </c>
+      <c r="B562">
+        <v>0.006209</v>
+      </c>
+      <c r="C562">
+        <v>0.000528</v>
+      </c>
+      <c r="D562">
+        <v>0.220506</v>
+      </c>
+      <c r="E562">
+        <v>1.382212</v>
+      </c>
+      <c r="F562">
+        <v>0.353835</v>
+      </c>
+      <c r="G562">
+        <v>1.736048</v>
+      </c>
+      <c r="H562">
+        <v>0.005995</v>
+      </c>
+      <c r="I562">
+        <v>0.012688</v>
+      </c>
+      <c r="J562">
+        <v>1.981975</v>
+      </c>
+    </row>
+    <row r="563" spans="1:10">
+      <c r="A563" s="6">
+        <v>43405</v>
+      </c>
+      <c r="B563">
+        <v>0.008164</v>
+      </c>
+      <c r="C563">
+        <v>1.1E-5</v>
+      </c>
+      <c r="D563">
+        <v>0.217799</v>
+      </c>
+      <c r="E563">
+        <v>1.37176</v>
+      </c>
+      <c r="F563">
+        <v>0.279834</v>
+      </c>
+      <c r="G563">
+        <v>1.651594</v>
+      </c>
+      <c r="H563">
+        <v>0.005247</v>
+      </c>
+      <c r="I563">
+        <v>0.013009</v>
+      </c>
+      <c r="J563">
+        <v>1.895825</v>
+      </c>
+    </row>
+    <row r="564" spans="1:10">
+      <c r="A564" s="6">
+        <v>43435</v>
+      </c>
+      <c r="B564">
+        <v>0.018334</v>
+      </c>
+      <c r="C564">
+        <v>0.000328</v>
+      </c>
+      <c r="D564">
+        <v>0.263577</v>
+      </c>
+      <c r="E564">
+        <v>1.333872</v>
+      </c>
+      <c r="F564">
+        <v>0.323119</v>
+      </c>
+      <c r="G564">
+        <v>1.656991</v>
+      </c>
+      <c r="H564">
+        <v>0.004343</v>
+      </c>
+      <c r="I564">
+        <v>0.013987</v>
+      </c>
+      <c r="J564">
+        <v>1.957559</v>
+      </c>
+    </row>
+    <row r="565" spans="1:10">
+      <c r="A565" s="6">
+        <v>43466</v>
+      </c>
+      <c r="B565">
+        <v>0.012843</v>
+      </c>
+      <c r="C565">
+        <v>6.9E-5</v>
+      </c>
+      <c r="D565">
+        <v>0.29811</v>
+      </c>
+      <c r="E565">
+        <v>1.41624</v>
+      </c>
+      <c r="F565">
+        <v>0.362987</v>
+      </c>
+      <c r="G565">
+        <v>1.779228</v>
+      </c>
+      <c r="H565">
+        <v>0.004634</v>
+      </c>
+      <c r="I565">
+        <v>0.016393</v>
+      </c>
+      <c r="J565">
+        <v>2.111277</v>
+      </c>
+    </row>
+    <row r="566" spans="1:10">
+      <c r="A566" s="6">
+        <v>43497</v>
+      </c>
+      <c r="B566">
+        <v>0.007369</v>
+      </c>
+      <c r="C566">
+        <v>1.7E-5</v>
+      </c>
+      <c r="D566">
+        <v>0.23915</v>
+      </c>
+      <c r="E566">
+        <v>1.131426</v>
+      </c>
+      <c r="F566">
+        <v>0.299076</v>
+      </c>
+      <c r="G566">
+        <v>1.430502</v>
+      </c>
+      <c r="H566">
+        <v>0.003101</v>
+      </c>
+      <c r="I566">
+        <v>0.01553</v>
+      </c>
+      <c r="J566">
+        <v>1.695668</v>
+      </c>
+    </row>
+    <row r="567" spans="1:10">
+      <c r="A567" s="6">
+        <v>43525</v>
+      </c>
+      <c r="B567">
+        <v>0.014506</v>
+      </c>
+      <c r="C567">
+        <v>6.5E-5</v>
+      </c>
+      <c r="D567">
+        <v>0.259313</v>
+      </c>
+      <c r="E567">
+        <v>1.272962</v>
+      </c>
+      <c r="F567">
+        <v>0.345854</v>
+      </c>
+      <c r="G567">
+        <v>1.618816</v>
+      </c>
+      <c r="H567">
+        <v>0.006123</v>
+      </c>
+      <c r="I567">
+        <v>0.016889</v>
+      </c>
+      <c r="J567">
+        <v>1.915713</v>
+      </c>
+    </row>
+    <row r="568" spans="1:10">
+      <c r="A568" s="6">
+        <v>43556</v>
+      </c>
+      <c r="B568">
+        <v>0.011032</v>
+      </c>
+      <c r="C568">
+        <v>0.000543</v>
+      </c>
+      <c r="D568">
+        <v>0.211723</v>
+      </c>
+      <c r="E568">
+        <v>1.280252</v>
+      </c>
+      <c r="F568">
+        <v>0.40096</v>
+      </c>
+      <c r="G568">
+        <v>1.681212</v>
+      </c>
+      <c r="H568">
+        <v>0.005524</v>
+      </c>
+      <c r="I568">
+        <v>0.014859</v>
+      </c>
+      <c r="J568">
+        <v>1.924893</v>
+      </c>
+    </row>
+    <row r="569" spans="1:10">
+      <c r="A569" s="6">
+        <v>43586</v>
+      </c>
+      <c r="B569">
+        <v>0.008379</v>
+      </c>
+      <c r="C569">
+        <v>0.00043</v>
+      </c>
+      <c r="D569">
+        <v>0.212842</v>
+      </c>
+      <c r="E569">
+        <v>1.348043</v>
+      </c>
+      <c r="F569">
+        <v>0.441993</v>
+      </c>
+      <c r="G569">
+        <v>1.790035</v>
+      </c>
+      <c r="H569">
+        <v>0.005055</v>
+      </c>
+      <c r="I569">
+        <v>0.016116</v>
+      </c>
+      <c r="J569">
+        <v>2.032857</v>
+      </c>
+    </row>
+    <row r="570" spans="1:10">
+      <c r="A570" s="6">
+        <v>43617</v>
+      </c>
+      <c r="B570">
+        <v>0.013559</v>
+      </c>
+      <c r="C570">
+        <v>1.9E-5</v>
+      </c>
+      <c r="D570">
+        <v>0.206192</v>
+      </c>
+      <c r="E570">
+        <v>1.301465</v>
+      </c>
+      <c r="F570">
+        <v>0.33627</v>
+      </c>
+      <c r="G570">
+        <v>1.637735</v>
+      </c>
+      <c r="H570">
+        <v>0.006957</v>
+      </c>
+      <c r="I570">
+        <v>0.017593</v>
+      </c>
+      <c r="J570">
+        <v>1.882055</v>
+      </c>
+    </row>
+    <row r="571" spans="1:10">
+      <c r="A571" s="6">
+        <v>43647</v>
+      </c>
+      <c r="B571">
+        <v>0.010511</v>
+      </c>
+      <c r="C571">
+        <v>1.5E-5</v>
+      </c>
+      <c r="D571">
+        <v>0.236168</v>
+      </c>
+      <c r="E571">
+        <v>1.306052</v>
+      </c>
+      <c r="F571">
+        <v>0.435821</v>
+      </c>
+      <c r="G571">
+        <v>1.741873</v>
+      </c>
+      <c r="H571">
+        <v>0.006679</v>
+      </c>
+      <c r="I571">
+        <v>0.019252</v>
+      </c>
+      <c r="J571">
+        <v>2.014497</v>
+      </c>
+    </row>
+    <row r="572" spans="1:10">
+      <c r="A572" s="6">
+        <v>43678</v>
+      </c>
+      <c r="B572">
+        <v>0.010668</v>
+      </c>
+      <c r="C572">
+        <v>0.000563</v>
+      </c>
+      <c r="D572">
+        <v>0.225578</v>
+      </c>
+      <c r="E572">
+        <v>1.307783</v>
+      </c>
+      <c r="F572">
+        <v>0.403433</v>
+      </c>
+      <c r="G572">
+        <v>1.711216</v>
+      </c>
+      <c r="H572">
+        <v>0.005145</v>
+      </c>
+      <c r="I572">
+        <v>0.020011</v>
+      </c>
+      <c r="J572">
+        <v>1.973182</v>
+      </c>
+    </row>
+    <row r="573" spans="1:10">
+      <c r="A573" s="6">
+        <v>43709</v>
+      </c>
+      <c r="B573">
+        <v>0.013385</v>
+      </c>
+      <c r="C573">
+        <v>0.000165</v>
+      </c>
+      <c r="D573">
+        <v>0.213494</v>
+      </c>
+      <c r="E573">
+        <v>1.180616</v>
+      </c>
+      <c r="F573">
+        <v>0.351319</v>
+      </c>
+      <c r="G573">
+        <v>1.531935</v>
+      </c>
+      <c r="H573">
+        <v>0.007474</v>
+      </c>
+      <c r="I573">
+        <v>0.018059</v>
+      </c>
+      <c r="J573">
+        <v>1.784512</v>
+      </c>
+    </row>
+    <row r="574" spans="1:10">
+      <c r="A574" s="6">
+        <v>43739</v>
+      </c>
+      <c r="B574">
+        <v>0.015262</v>
+      </c>
+      <c r="C574">
+        <v>0.000469</v>
+      </c>
+      <c r="D574">
+        <v>0.215801</v>
+      </c>
+      <c r="E574">
+        <v>1.17578</v>
+      </c>
+      <c r="F574">
+        <v>0.387666</v>
+      </c>
+      <c r="G574">
+        <v>1.563446</v>
+      </c>
+      <c r="H574">
+        <v>0.007324</v>
+      </c>
+      <c r="I574">
+        <v>0.012492</v>
+      </c>
+      <c r="J574">
+        <v>1.814793</v>
+      </c>
+    </row>
+    <row r="575" spans="1:10">
+      <c r="A575" s="6">
+        <v>43770</v>
+      </c>
+      <c r="B575">
+        <v>0.009579</v>
+      </c>
+      <c r="C575">
+        <v>0.000504</v>
+      </c>
+      <c r="D575">
+        <v>0.229359</v>
+      </c>
+      <c r="E575">
+        <v>1.060002</v>
+      </c>
+      <c r="F575">
+        <v>0.360991</v>
+      </c>
+      <c r="G575">
+        <v>1.420994</v>
+      </c>
+      <c r="H575">
+        <v>0.006329</v>
+      </c>
+      <c r="I575">
+        <v>0.016512</v>
+      </c>
+      <c r="J575">
+        <v>1.683276</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10">
+      <c r="A576" s="6">
+        <v>43800</v>
+      </c>
+      <c r="B576">
+        <v>0.010585</v>
+      </c>
+      <c r="C576">
+        <v>9.0E-6</v>
+      </c>
+      <c r="D576">
+        <v>0.262454</v>
+      </c>
+      <c r="E576">
+        <v>1.286387</v>
+      </c>
+      <c r="F576">
+        <v>0.387429</v>
+      </c>
+      <c r="G576">
+        <v>1.673816</v>
+      </c>
+      <c r="H576">
+        <v>0.00702</v>
+      </c>
+      <c r="I576">
+        <v>0.017782</v>
+      </c>
+      <c r="J576">
+        <v>1.971665</v>
+      </c>
+    </row>
+    <row r="577" spans="1:10">
+      <c r="A577" s="6">
+        <v>43831</v>
+      </c>
+      <c r="B577">
+        <v>0.011001</v>
+      </c>
+      <c r="C577">
+        <v>7.1E-5</v>
+      </c>
+      <c r="D577">
+        <v>0.268675</v>
+      </c>
+      <c r="E577">
+        <v>1.206878</v>
+      </c>
+      <c r="F577">
+        <v>0.360895</v>
+      </c>
+      <c r="G577">
+        <v>1.567772</v>
+      </c>
+      <c r="H577">
+        <v>0.005737</v>
+      </c>
+      <c r="I577">
+        <v>0.015847</v>
+      </c>
+      <c r="J577">
+        <v>1.869103</v>
+      </c>
+    </row>
+    <row r="578" spans="1:10">
+      <c r="A578" s="6">
+        <v>43862</v>
+      </c>
+      <c r="B578">
+        <v>0.007054</v>
+      </c>
+      <c r="C578">
+        <v>4.8E-5</v>
+      </c>
+      <c r="D578">
+        <v>0.244117</v>
+      </c>
+      <c r="E578">
+        <v>1.14854</v>
+      </c>
+      <c r="F578">
+        <v>0.3024</v>
+      </c>
+      <c r="G578">
+        <v>1.450939</v>
+      </c>
+      <c r="H578">
+        <v>0.00474</v>
+      </c>
+      <c r="I578">
+        <v>0.016706</v>
+      </c>
+      <c r="J578">
+        <v>1.723604</v>
+      </c>
+    </row>
+    <row r="579" spans="1:10">
+      <c r="A579" s="6">
+        <v>43891</v>
+      </c>
+      <c r="B579">
+        <v>0.009473</v>
+      </c>
+      <c r="C579">
+        <v>2.2E-5</v>
+      </c>
+      <c r="D579">
+        <v>0.222514</v>
+      </c>
+      <c r="E579">
+        <v>1.185725</v>
+      </c>
+      <c r="F579">
+        <v>0.341985</v>
+      </c>
+      <c r="G579">
+        <v>1.527709</v>
+      </c>
+      <c r="H579">
+        <v>0.005156</v>
+      </c>
+      <c r="I579">
+        <v>0.016735</v>
+      </c>
+      <c r="J579">
+        <v>1.781609</v>
+      </c>
+    </row>
+    <row r="580" spans="1:10">
+      <c r="A580" s="6">
+        <v>43922</v>
+      </c>
+      <c r="B580">
+        <v>0.007496</v>
+      </c>
+      <c r="C580">
+        <v>0.000117</v>
+      </c>
+      <c r="D580">
+        <v>0.198112</v>
+      </c>
+      <c r="E580">
+        <v>1.005935</v>
+      </c>
+      <c r="F580">
+        <v>0.274473</v>
+      </c>
+      <c r="G580">
+        <v>1.280408</v>
+      </c>
+      <c r="H580">
+        <v>0.006922</v>
+      </c>
+      <c r="I580">
+        <v>0.015854</v>
+      </c>
+      <c r="J580">
+        <v>1.508908</v>
       </c>
     </row>
   </sheetData>
@@ -18021,7 +18789,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A13" sqref="A13"/>
@@ -20315,31 +21083,95 @@
         <v>2017</v>
       </c>
       <c r="B81">
-        <v>0.167054</v>
+        <v>0.167124</v>
       </c>
       <c r="C81">
         <v>0.00145</v>
       </c>
       <c r="D81">
-        <v>3.11845</v>
+        <v>3.109057</v>
       </c>
       <c r="E81">
-        <v>17.502883</v>
+        <v>17.597454</v>
       </c>
       <c r="F81">
-        <v>4.253518</v>
+        <v>4.276752</v>
       </c>
       <c r="G81">
-        <v>21.756402</v>
+        <v>21.874205</v>
       </c>
       <c r="H81">
-        <v>0.082558</v>
+        <v>0.08135</v>
       </c>
       <c r="I81">
         <v>0.224117</v>
       </c>
       <c r="J81">
-        <v>25.350031</v>
+        <v>25.457303</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="7">
+        <v>2018</v>
+      </c>
+      <c r="B82">
+        <v>0.121554</v>
+      </c>
+      <c r="C82">
+        <v>0.002895</v>
+      </c>
+      <c r="D82">
+        <v>2.961068</v>
+      </c>
+      <c r="E82">
+        <v>17.191582</v>
+      </c>
+      <c r="F82">
+        <v>4.308952</v>
+      </c>
+      <c r="G82">
+        <v>21.500533</v>
+      </c>
+      <c r="H82">
+        <v>0.048437</v>
+      </c>
+      <c r="I82">
+        <v>0.198785</v>
+      </c>
+      <c r="J82">
+        <v>24.833272</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="7">
+        <v>2019</v>
+      </c>
+      <c r="B83">
+        <v>0.137678</v>
+      </c>
+      <c r="C83">
+        <v>0.002868</v>
+      </c>
+      <c r="D83">
+        <v>2.810182</v>
+      </c>
+      <c r="E83">
+        <v>15.067008</v>
+      </c>
+      <c r="F83">
+        <v>4.5138</v>
+      </c>
+      <c r="G83">
+        <v>19.580808</v>
+      </c>
+      <c r="H83">
+        <v>0.071365</v>
+      </c>
+      <c r="I83">
+        <v>0.201487</v>
+      </c>
+      <c r="J83">
+        <v>22.804389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>